<commit_message>
Fixed issue with upload errors and run model errors not being s displayed
</commit_message>
<xml_diff>
--- a/yw_react_fe/yw-fe/testFiles/yw_reference_tables (1).xlsx
+++ b/yw_react_fe/yw-fe/testFiles/yw_reference_tables (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/dev/YW-sludge-modelling-app/yw_react_fe/yw-fe/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2180016E-15D0-1E46-A48C-8701F24EA7FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD8DB4E-6BED-A643-AA00-814E33C6C03C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="23240" windowHeight="12560" firstSheet="1" activeTab="9" xr2:uid="{455B0008-4095-42C4-8FA9-2EDAC3BC0A90}"/>
+    <workbookView xWindow="17420" yWindow="12320" windowWidth="23240" windowHeight="12560" xr2:uid="{455B0008-4095-42C4-8FA9-2EDAC3BC0A90}"/>
   </bookViews>
   <sheets>
     <sheet name="Volumes" sheetId="10" r:id="rId1"/>
@@ -581,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB8528B0-FFA9-4A90-988D-6EAEC0010E0D}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -622,7 +622,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>0.02</v>
@@ -821,7 +821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30ADBD12-0DE1-42EB-8D5A-84BF08F8492F}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>

</xml_diff>